<commit_message>
Included changes without front-page
</commit_message>
<xml_diff>
--- a/R/Results.xlsx
+++ b/R/Results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="700" windowWidth="29180" windowHeight="16660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="18860" yWindow="700" windowWidth="18240" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Most frequent items" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>bbs</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t xml:space="preserve">{local, news} =&gt; {frontpage} </t>
+  </si>
+  <si>
+    <t>Without front page</t>
   </si>
 </sst>
 </file>
@@ -277,10 +280,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -379,7 +394,7 @@
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="95">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -421,6 +436,12 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -461,6 +482,12 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -499,6 +526,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -593,11 +621,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2091369224"/>
-        <c:axId val="-2130187336"/>
+        <c:axId val="-2064881800"/>
+        <c:axId val="-2065251368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2091369224"/>
+        <c:axId val="-2064881800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,12 +647,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2130187336"/>
+        <c:crossAx val="-2065251368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -632,7 +661,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130187336"/>
+        <c:axId val="-2065251368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -655,13 +684,228 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2091369224"/>
+        <c:crossAx val="-2064881800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="117"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="17"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Itemset Size Distribution</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>without</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> "frontpage"</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Itemset Width Distribution'!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Itemset Width Distribution'!$C$23:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.72660673300455</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.177677247918751</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0602243152532303</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0219379076225509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00841366936777031</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00311836331740653</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00132419598691765</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.000447802883968804</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.000164046601057879</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.32043030457986E-5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.66021515228993E-5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.43369192048321E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.47789730682774E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2073752952"/>
+        <c:axId val="-2132690552"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2073752952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Itemset Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2132690552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2132690552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Support (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2073752952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -705,6 +949,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1035,15 +1311,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1190,9 +1466,150 @@
         <v>2.057658E-3</v>
       </c>
     </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4">
+        <v>0.25895358299999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0.147133815</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4">
+        <v>0.129582846</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="4">
+        <v>0.124182098</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="4">
+        <v>0.120735684</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="4">
+        <v>0.11748236200000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="4">
+        <v>0.11538906</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="4">
+        <v>0.106990985</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="4">
+        <v>0.10094220499999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="4">
+        <v>6.4503247E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="4">
+        <v>3.6387759999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34" s="4">
+        <v>3.5631479000000001E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="4">
+        <v>2.9110207999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1.8493026999999999E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="4">
+        <v>5.0994059999999999E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1.224384E-3</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:B18">
-    <sortCondition descending="1" ref="B2:B18"/>
+  <sortState ref="A23:B38">
+    <sortCondition descending="1" ref="B23:B38"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1206,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" activeCellId="1" sqref="A1:A18 C1:C18"/>
+    <sheetView topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1437,6 +1854,197 @@
         <f>SUM(B2:B18)</f>
         <v>989818</v>
       </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>491649</v>
+      </c>
+      <c r="C23" s="3">
+        <f>B23/$B$36</f>
+        <v>0.72660673300455048</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1">
+        <v>120223</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" ref="C24:C35" si="1">B24/$B$36</f>
+        <v>0.17767724791875111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1">
+        <v>40750</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="1"/>
+        <v>6.0224315253230312E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>14844</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="1"/>
+        <v>2.1937907622550941E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5693</v>
+      </c>
+      <c r="C27" s="3">
+        <f t="shared" si="1"/>
+        <v>8.4136693677703111E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2110</v>
+      </c>
+      <c r="C28" s="3">
+        <f t="shared" si="1"/>
+        <v>3.1183633174065267E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1">
+        <v>896</v>
+      </c>
+      <c r="C29" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3241959869176531E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1">
+        <v>303</v>
+      </c>
+      <c r="C30" s="3">
+        <f t="shared" si="1"/>
+        <v>4.4780288396880453E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1">
+        <v>111</v>
+      </c>
+      <c r="C31" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6404660105787889E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1">
+        <v>36</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" si="1"/>
+        <v>5.320430304579856E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>11</v>
+      </c>
+      <c r="B33" s="1">
+        <v>18</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="1"/>
+        <v>2.660215152289928E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="1"/>
+        <v>4.4336919204832136E-6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>13</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="1"/>
+        <v>1.4778973068277378E-6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="B36" s="2">
+        <f>SUM(B23:B35)</f>
+        <v>676637</v>
+      </c>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37" s="1"/>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1454,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added write-up on association analysis and visualization for project report.
</commit_message>
<xml_diff>
--- a/R/Results.xlsx
+++ b/R/Results.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18860" yWindow="700" windowWidth="18240" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="-200" yWindow="1080" windowWidth="24920" windowHeight="16660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Most frequent items" sheetId="1" r:id="rId1"/>
     <sheet name="Itemset Width Distribution" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -503,33 +504,14 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="117"/>
+      <c14:style val="101"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="17"/>
+      <c:style val="1"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Itemset Size Distribution</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -550,6 +532,9 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
@@ -614,18 +599,18 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2064881800"/>
-        <c:axId val="-2065251368"/>
+        <c:gapWidth val="75"/>
+        <c:axId val="-2143211080"/>
+        <c:axId val="2090731608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2064881800"/>
+        <c:axId val="-2143211080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,7 +638,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2065251368"/>
+        <c:crossAx val="2090731608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -661,17 +646,16 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065251368"/>
+        <c:axId val="2090731608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" vert="horz"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
@@ -688,10 +672,10 @@
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2064881800"/>
+        <c:crossAx val="-2143211080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -835,11 +819,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2073752952"/>
-        <c:axId val="-2132690552"/>
+        <c:axId val="2090804888"/>
+        <c:axId val="2090810392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2073752952"/>
+        <c:axId val="2090804888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,7 +851,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132690552"/>
+        <c:crossAx val="2090810392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -875,7 +859,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132690552"/>
+        <c:axId val="2090810392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +889,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073752952"/>
+        <c:crossAx val="2090804888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1313,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1625,7 +1609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="D28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -2617,4 +2601,21 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>